<commit_message>
Update files and folders
</commit_message>
<xml_diff>
--- a/Population estimates strategy.xlsx
+++ b/Population estimates strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vishalsingh/[Research]/PhD/R/Population estimates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB246FF-78B7-EB4B-87EC-20B3EB6A861A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BC6187-0561-5945-8C87-10EF48EC0AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="500" windowWidth="43400" windowHeight="28300" xr2:uid="{0ED177E6-E686-E04B-823F-D7CF20C3B323}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{0ED177E6-E686-E04B-823F-D7CF20C3B323}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2024,7 +2024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978BF1E3-311D-1E4E-B87D-2B494F7C0D2E}">
   <dimension ref="B1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Update strategy and analysis files
</commit_message>
<xml_diff>
--- a/Population estimates strategy.xlsx
+++ b/Population estimates strategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vishalsingh/[Research]/PhD/R/Population estimates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BC6187-0561-5945-8C87-10EF48EC0AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE93966-0CEA-E24B-81F1-CF26F9A5A879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{0ED177E6-E686-E04B-823F-D7CF20C3B323}"/>
   </bookViews>
@@ -154,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -267,6 +267,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -613,58 +620,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -672,18 +643,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -735,19 +694,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -797,6 +744,63 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2035,721 +2039,726 @@
   <sheetData>
     <row r="1" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="22" x14ac:dyDescent="0.2">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="45"/>
+      <c r="G2" s="54"/>
     </row>
     <row r="3" spans="2:7" ht="22" x14ac:dyDescent="0.2">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="27" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="100" x14ac:dyDescent="0.2">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="29" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="50"/>
-      <c r="C5" s="31">
+      <c r="B5" s="30"/>
+      <c r="C5" s="15">
         <v>1995</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="14">
         <v>1995</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="11">
         <v>1995</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="8">
         <v>1995</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="31">
         <v>1995</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="52"/>
-      <c r="C6" s="32">
+      <c r="B6" s="32"/>
+      <c r="C6" s="16">
         <v>1996</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="13">
         <v>1996</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="12">
         <v>1996</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="9">
         <v>1996</v>
       </c>
-      <c r="G6" s="53">
+      <c r="G6" s="33">
         <v>1996</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="52"/>
-      <c r="C7" s="32">
+      <c r="B7" s="32"/>
+      <c r="C7" s="16">
         <v>1997</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="13">
         <v>1997</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="12">
         <v>1997</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="9">
         <v>1997</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="33">
         <v>1997</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="52"/>
-      <c r="C8" s="32">
+      <c r="B8" s="32"/>
+      <c r="C8" s="16">
         <v>1998</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="13">
         <v>1998</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="12">
         <v>1998</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="9">
         <v>1998</v>
       </c>
-      <c r="G8" s="53">
+      <c r="G8" s="33">
         <v>1998</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="52"/>
-      <c r="C9" s="32">
+      <c r="B9" s="32"/>
+      <c r="C9" s="16">
         <v>1999</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="13">
         <v>1999</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="12">
         <v>1999</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="9">
         <v>1999</v>
       </c>
-      <c r="G9" s="53">
+      <c r="G9" s="33">
         <v>1999</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="52"/>
-      <c r="C10" s="32">
+      <c r="B10" s="32"/>
+      <c r="C10" s="16">
         <v>2000</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="13">
         <v>2000</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="12">
         <v>2000</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="9">
         <v>2000</v>
       </c>
-      <c r="G10" s="53">
+      <c r="G10" s="33">
         <v>2000</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="54">
+      <c r="B11" s="34">
         <v>2001</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="17">
         <v>2001</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="13">
         <v>2001</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="12">
         <v>2001</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="9">
         <v>2001</v>
       </c>
-      <c r="G11" s="53">
+      <c r="G11" s="33">
         <v>2001</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="54">
+      <c r="B12" s="34">
         <v>2002</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="17">
         <v>2002</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="13">
         <v>2002</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="12">
         <v>2002</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="9">
         <v>2002</v>
       </c>
-      <c r="G12" s="53">
+      <c r="G12" s="33">
         <v>2002</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="54">
+      <c r="B13" s="34">
         <v>2003</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="17">
         <v>2003</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="13">
         <v>2003</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="12">
         <v>2003</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="9">
         <v>2003</v>
       </c>
-      <c r="G13" s="53">
+      <c r="G13" s="33">
         <v>2003</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="54">
+      <c r="B14" s="34">
         <v>2004</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="17">
         <v>2004</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="13">
         <v>2004</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="12">
         <v>2004</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="9">
         <v>2004</v>
       </c>
-      <c r="G14" s="53">
+      <c r="G14" s="33">
         <v>2004</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="54">
+      <c r="B15" s="34">
         <v>2005</v>
       </c>
-      <c r="C15" s="33">
+      <c r="C15" s="17">
         <v>2005</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="13">
         <v>2005</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="12">
         <v>2005</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="9">
         <v>2005</v>
       </c>
-      <c r="G15" s="53">
+      <c r="G15" s="33">
         <v>2005</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="54">
+      <c r="B16" s="34">
         <v>2006</v>
       </c>
-      <c r="C16" s="33">
+      <c r="C16" s="17">
         <v>2006</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="13">
         <v>2006</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="12">
         <v>2006</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="9">
         <v>2006</v>
       </c>
-      <c r="G16" s="53">
+      <c r="G16" s="33">
         <v>2006</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="54">
+      <c r="B17" s="34">
         <v>2007</v>
       </c>
-      <c r="C17" s="33">
+      <c r="C17" s="17">
         <v>2007</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="13">
         <v>2007</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="12">
         <v>2007</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="9">
         <v>2007</v>
       </c>
-      <c r="G17" s="53">
+      <c r="G17" s="33">
         <v>2007</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="54">
+      <c r="B18" s="34">
         <v>2008</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C18" s="17">
         <v>2008</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="13">
         <v>2008</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="12">
         <v>2008</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="9">
         <v>2008</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="33">
         <v>2008</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="54">
+      <c r="B19" s="34">
         <v>2009</v>
       </c>
-      <c r="C19" s="33">
+      <c r="C19" s="17">
         <v>2009</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="13">
         <v>2009</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="12">
         <v>2009</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="9">
         <v>2009</v>
       </c>
-      <c r="G19" s="53">
+      <c r="G19" s="33">
         <v>2009</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="54">
+      <c r="B20" s="34">
         <v>2010</v>
       </c>
-      <c r="C20" s="33">
+      <c r="C20" s="17">
         <v>2010</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="13">
         <v>2010</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="12">
         <v>2010</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="9">
         <v>2010</v>
       </c>
-      <c r="G20" s="53">
+      <c r="G20" s="33">
         <v>2010</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="54">
+      <c r="B21" s="34">
         <v>2011</v>
       </c>
-      <c r="C21" s="33">
+      <c r="C21" s="17">
         <v>2011</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="13">
         <v>2011</v>
       </c>
-      <c r="E21" s="29">
+      <c r="E21" s="13">
         <v>2011</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="9">
         <v>2011</v>
       </c>
-      <c r="G21" s="53">
+      <c r="G21" s="33">
         <v>2011</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="54">
+      <c r="B22" s="34">
         <v>2012</v>
       </c>
-      <c r="C22" s="33">
+      <c r="C22" s="17">
         <v>2012</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="13">
         <v>2012</v>
       </c>
-      <c r="E22" s="29">
+      <c r="E22" s="13">
         <v>2012</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="9">
         <v>2012</v>
       </c>
-      <c r="G22" s="53">
+      <c r="G22" s="33">
         <v>2012</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="54">
+      <c r="B23" s="34">
         <v>2013</v>
       </c>
-      <c r="C23" s="33">
+      <c r="C23" s="17">
         <v>2013</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="13">
         <v>2013</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23" s="13">
         <v>2013</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="9">
         <v>2013</v>
       </c>
-      <c r="G23" s="53">
+      <c r="G23" s="33">
         <v>2013</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="54">
+      <c r="B24" s="34">
         <v>2014</v>
       </c>
-      <c r="C24" s="33">
+      <c r="C24" s="17">
         <v>2014</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="13">
         <v>2014</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="13">
         <v>2014</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="9">
         <v>2014</v>
       </c>
-      <c r="G24" s="53">
+      <c r="G24" s="33">
         <v>2014</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="54">
+      <c r="B25" s="34">
         <v>2015</v>
       </c>
-      <c r="C25" s="33">
+      <c r="C25" s="17">
         <v>2015</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25" s="13">
         <v>2015</v>
       </c>
-      <c r="E25" s="29">
+      <c r="E25" s="13">
         <v>2015</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="9">
         <v>2015</v>
       </c>
-      <c r="G25" s="53">
+      <c r="G25" s="33">
         <v>2015</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="54">
+      <c r="B26" s="34">
         <v>2016</v>
       </c>
-      <c r="C26" s="33">
+      <c r="C26" s="17">
         <v>2016</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="13">
         <v>2016</v>
       </c>
-      <c r="E26" s="29">
+      <c r="E26" s="13">
         <v>2016</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="10">
         <v>2016</v>
       </c>
-      <c r="G26" s="55">
+      <c r="G26" s="35">
         <v>2016</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="54">
+      <c r="B27" s="34">
         <v>2017</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C27" s="17">
         <v>2017</v>
       </c>
-      <c r="D27" s="29">
+      <c r="D27" s="13">
         <v>2017</v>
       </c>
-      <c r="E27" s="29">
+      <c r="E27" s="13">
         <v>2017</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="9">
         <v>2017</v>
       </c>
-      <c r="G27" s="53">
+      <c r="G27" s="33">
         <v>2017</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="54">
+      <c r="B28" s="34">
         <v>2018</v>
       </c>
-      <c r="C28" s="33">
+      <c r="C28" s="17">
         <v>2018</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="13">
         <v>2018</v>
       </c>
-      <c r="E28" s="29">
+      <c r="E28" s="13">
         <v>2018</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="9">
         <v>2018</v>
       </c>
-      <c r="G28" s="53">
+      <c r="G28" s="33">
         <v>2018</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="54">
+      <c r="B29" s="34">
         <v>2019</v>
       </c>
-      <c r="C29" s="33">
+      <c r="C29" s="17">
         <v>2019</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="13">
         <v>2019</v>
       </c>
-      <c r="E29" s="29">
+      <c r="E29" s="13">
         <v>2019</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="9">
         <v>2019</v>
       </c>
-      <c r="G29" s="53">
+      <c r="G29" s="33">
         <v>2019</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="54">
+      <c r="B30" s="34">
         <v>2020</v>
       </c>
-      <c r="C30" s="33">
+      <c r="C30" s="17">
         <v>2020</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="13">
         <v>2020</v>
       </c>
-      <c r="E30" s="29">
+      <c r="E30" s="13">
         <v>2020</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="9">
         <v>2020</v>
       </c>
-      <c r="G30" s="53">
+      <c r="G30" s="33">
         <v>2020</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="54">
+      <c r="B31" s="34">
         <v>2021</v>
       </c>
-      <c r="C31" s="33">
+      <c r="C31" s="17">
         <v>2021</v>
       </c>
-      <c r="D31" s="29">
+      <c r="D31" s="13">
         <v>2021</v>
       </c>
-      <c r="E31" s="29">
+      <c r="E31" s="13">
         <v>2021</v>
       </c>
-      <c r="F31" s="26">
+      <c r="F31" s="10">
         <v>2021</v>
       </c>
-      <c r="G31" s="53">
+      <c r="G31" s="33">
         <v>2021</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="54">
+      <c r="B32" s="34">
         <v>2022</v>
       </c>
-      <c r="C32" s="33">
+      <c r="C32" s="17">
         <v>2022</v>
       </c>
-      <c r="D32" s="29">
+      <c r="D32" s="13">
         <v>2022</v>
       </c>
-      <c r="E32" s="29">
+      <c r="E32" s="13">
         <v>2022</v>
       </c>
-      <c r="F32" s="25">
+      <c r="F32" s="9">
         <v>2022</v>
       </c>
-      <c r="G32" s="53">
+      <c r="G32" s="33">
         <v>2022</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="56">
+      <c r="B33" s="36">
         <v>2023</v>
       </c>
-      <c r="C33" s="57">
+      <c r="C33" s="37">
         <v>2023</v>
       </c>
-      <c r="D33" s="58">
+      <c r="D33" s="38">
         <v>2023</v>
       </c>
-      <c r="E33" s="58">
+      <c r="E33" s="38">
         <v>2023</v>
       </c>
-      <c r="F33" s="59">
+      <c r="F33" s="39">
         <v>2023</v>
       </c>
-      <c r="G33" s="60">
+      <c r="G33" s="40">
         <v>2023</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="17" t="s">
+      <c r="D35" s="46"/>
+      <c r="E35" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="G35" s="4"/>
+      <c r="G35" s="46"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="20" t="s">
+      <c r="D36" s="56"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="21"/>
+      <c r="G36" s="48"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="20" t="s">
+      <c r="D37" s="58"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="G37" s="21"/>
+      <c r="G37" s="48"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="20" t="s">
+      <c r="D38" s="60"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G38" s="21"/>
+      <c r="G38" s="48"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="16"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="22" t="s">
+      <c r="D39" s="44"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G39" s="23"/>
-    </row>
-    <row r="41" spans="2:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="B41" s="61"/>
-      <c r="C41" s="61" t="s">
+      <c r="G39" s="50"/>
+    </row>
+    <row r="41" spans="2:7" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="B41" s="41"/>
+      <c r="C41" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="61" t="s">
+      <c r="D41" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="E41" s="61" t="s">
+      <c r="E41" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F41" s="61" t="s">
+      <c r="F41" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="G41" s="61" t="s">
+      <c r="G41" s="41" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="F35:G35"/>
@@ -2757,11 +2766,6 @@
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="F39:G39"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>